<commit_message>
Changes in xml file 11 and in execution order file
</commit_message>
<xml_diff>
--- a/Scenarios_Execution_Order.xlsx
+++ b/Scenarios_Execution_Order.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Automation Projects\Vidhisinghania_Ar\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18450" windowHeight="9870" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12420" windowHeight="9870" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="New_Actual_Series" sheetId="1" r:id="rId1"/>
@@ -18,6 +13,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="980">
   <si>
     <t>SI.No</t>
   </si>
@@ -3160,7 +3156,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3287,6 +3283,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -3393,7 +3395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3617,6 +3619,12 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7069,8 +7077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BY172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10253,11 +10261,14 @@
       <c r="B71" s="93">
         <v>70</v>
       </c>
-      <c r="C71" s="27" t="s">
+      <c r="C71" s="88" t="s">
         <v>957</v>
       </c>
-      <c r="D71" s="27" t="s">
+      <c r="D71" s="88" t="s">
         <v>960</v>
+      </c>
+      <c r="E71" s="64" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10267,11 +10278,14 @@
       <c r="B72" s="93">
         <v>71</v>
       </c>
-      <c r="C72" s="27" t="s">
+      <c r="C72" s="88" t="s">
         <v>958</v>
       </c>
-      <c r="D72" s="27" t="s">
+      <c r="D72" s="88" t="s">
         <v>499</v>
+      </c>
+      <c r="E72" s="64" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="120" x14ac:dyDescent="0.25">
@@ -10927,7 +10941,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="95" t="s">
         <v>932</v>
       </c>
@@ -10941,7 +10955,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="95" t="s">
         <v>932</v>
       </c>
@@ -10955,7 +10969,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="95" t="s">
         <v>932</v>
       </c>
@@ -10969,7 +10983,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="95" t="s">
         <v>932</v>
       </c>
@@ -10983,7 +10997,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="95" t="s">
         <v>932</v>
       </c>
@@ -10997,7 +11011,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="95" t="s">
         <v>932</v>
       </c>
@@ -11011,7 +11025,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="95" t="s">
         <v>932</v>
       </c>
@@ -11025,7 +11039,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="95" t="s">
         <v>932</v>
       </c>
@@ -11039,7 +11053,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="95" t="s">
         <v>932</v>
       </c>
@@ -11053,7 +11067,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="95" t="s">
         <v>932</v>
       </c>
@@ -11067,7 +11081,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="95" t="s">
         <v>932</v>
       </c>
@@ -11081,7 +11095,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="95" t="s">
         <v>932</v>
       </c>
@@ -11095,7 +11109,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="95" t="s">
         <v>932</v>
       </c>
@@ -11109,7 +11123,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="95" t="s">
         <v>932</v>
       </c>
@@ -11123,7 +11137,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="127" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="10" t="s">
         <v>932</v>
       </c>
@@ -11137,35 +11151,41 @@
         <v>972</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
         <v>932</v>
       </c>
       <c r="B128" s="93">
         <v>127</v>
       </c>
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="99" t="s">
         <v>507</v>
       </c>
       <c r="D128" s="62" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E128" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>932</v>
       </c>
       <c r="B129" s="93">
         <v>128</v>
       </c>
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="99" t="s">
         <v>508</v>
       </c>
       <c r="D129" s="62" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="E129" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A130" s="10" t="s">
         <v>932</v>
       </c>
@@ -11179,21 +11199,24 @@
         <v>512</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>932</v>
       </c>
       <c r="B131" s="93">
         <v>130</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="100" t="s">
         <v>513</v>
       </c>
       <c r="D131" s="62" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
         <v>932</v>
       </c>
@@ -11207,21 +11230,24 @@
         <v>516</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="10" t="s">
         <v>932</v>
       </c>
       <c r="B133" s="93">
         <v>132</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="100" t="s">
         <v>517</v>
       </c>
       <c r="D133" s="62" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
         <v>932</v>
       </c>
@@ -11235,21 +11261,24 @@
         <v>559</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="10" t="s">
         <v>932</v>
       </c>
       <c r="B135" s="93">
         <v>134</v>
       </c>
-      <c r="C135" s="81" t="s">
+      <c r="C135" s="99" t="s">
         <v>560</v>
       </c>
       <c r="D135" s="81" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E135" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="10" t="s">
         <v>933</v>
       </c>
@@ -11263,7 +11292,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="10" t="s">
         <v>933</v>
       </c>
@@ -11277,7 +11306,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="10" t="s">
         <v>933</v>
       </c>
@@ -11291,7 +11320,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="10" t="s">
         <v>933</v>
       </c>
@@ -11305,7 +11334,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="10" t="s">
         <v>933</v>
       </c>
@@ -11319,7 +11348,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="10" t="s">
         <v>933</v>
       </c>
@@ -11333,7 +11362,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="10" t="s">
         <v>933</v>
       </c>
@@ -11347,7 +11376,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="97" t="s">
         <v>933</v>
       </c>
@@ -11361,7 +11390,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="97" t="s">
         <v>933</v>
       </c>

</xml_diff>